<commit_message>
Update code woth ANova, First real draft
</commit_message>
<xml_diff>
--- a/Data_questionaire_finance_tracksyears.xlsx
+++ b/Data_questionaire_finance_tracksyears.xlsx
@@ -20,11 +20,8 @@
   </sheets>
   <definedNames>
     <definedName name="_xlchart.0" hidden="1">TracsYears!$AS$2:$AS$83</definedName>
-    <definedName name="_xlchart.1" hidden="1">TracsYears!$AS$2:$AS$83</definedName>
-    <definedName name="_xlchart.2" hidden="1">TracsYears!$AS$2:$AS$83</definedName>
-    <definedName name="_xlchart.3" hidden="1">TracsYears!$AS$2:$AS$83</definedName>
   </definedNames>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -18208,6 +18205,7 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -52834,8 +52832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AT88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA54" workbookViewId="0">
-      <selection activeCell="AR92" sqref="AR92"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>